<commit_message>
Ripetizione Test 36,39 aggiornata checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111AMGMEDICALX/D.EVO/DEVORIS/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111AMGMEDICALX/D.EVO/DEVORIS/1.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progetti\it-fse-accreditamento\GATEWAY\A1#111AMGMEDICALX\D.EVO\DEVORIS\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A491F3F-F768-4A06-A160-1D4FB6D0B667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04001D29-0D44-4F35-AB70-F69A7E66732D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -875,9 +875,6 @@
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t>2023-03-29T16:52:11Z</t>
-  </si>
-  <si>
     <t>Si</t>
   </si>
   <si>
@@ -1075,12 +1072,6 @@
     <t>2.16.840.1.113883.2.9.2.150.4.4.aa7cb8dd13f61c5aaee7421cbbe3c22d0d3e8e2c100245479d1f079532e8df0a.e0c74447c9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-06-22T12:11:10Z</t>
-  </si>
-  <si>
-    <t>dfc68f0d733e2a78</t>
-  </si>
-  <si>
     <t xml:space="preserve">Viene mostrato a video il messaggio di errore "TIME OUT VALIDAZIONE". Il medico può produrre il referto e l'invio al FSE rimarrà in coda fino al ripristino del servizio. </t>
   </si>
   <si>
@@ -1141,12 +1132,6 @@
     <t>Il Software non gestisce le sezioni opzionali</t>
   </si>
   <si>
-    <t>2583dd5a5e5def41</t>
-  </si>
-  <si>
-    <t>Campo token JWT non valido</t>
-  </si>
-  <si>
     <t>Viene mostrato a video un messaggio di errore contenente i campi "title" e "detail" della response e la sua interpretazione con le istruzioni per correggere l'errore. Il medico può produrre il referto ma per l'invio al FSE sarà necessario correggere l'errore</t>
   </si>
   <si>
@@ -1175,6 +1160,21 @@
   </si>
   <si>
     <t>Attenzione è obbligatorio valorizzare Il campo "Tipologia Campione"</t>
+  </si>
+  <si>
+    <t>d2368f4c1c49e9b2</t>
+  </si>
+  <si>
+    <t>Campo token JWT non valido, Il campo action_id non è corretto</t>
+  </si>
+  <si>
+    <t>44ceddc323217c6a</t>
+  </si>
+  <si>
+    <t>2023-06-27T09:38:10Z</t>
+  </si>
+  <si>
+    <t>2023-06-27T09:40:00Z</t>
   </si>
 </sst>
 </file>
@@ -2136,8 +2136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2156,17 +2156,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14.25" customHeight="1">
+    <row r="3" spans="1:1" ht="42" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="14.25" customHeight="1">
+    <row r="4" spans="1:1" ht="168.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="14.25" customHeight="1">
+    <row r="5" spans="1:1" ht="67.5" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2189,12 +2189,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="14.25" customHeight="1">
+    <row r="10" spans="1:1" ht="75.75" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="14.25" customHeight="1">
+    <row r="11" spans="1:1" ht="57" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -4297,10 +4297,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:T606"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G26" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4347,7 +4348,7 @@
       </c>
       <c r="B2" s="60"/>
       <c r="C2" s="61" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D2" s="60"/>
       <c r="F2" s="12"/>
@@ -4372,7 +4373,7 @@
       </c>
       <c r="B3" s="63"/>
       <c r="C3" s="68" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D3" s="69"/>
       <c r="F3" s="12"/>
@@ -4395,7 +4396,7 @@
       <c r="A4" s="64"/>
       <c r="B4" s="65"/>
       <c r="C4" s="70" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D4" s="60"/>
       <c r="E4" s="4"/>
@@ -4557,7 +4558,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="210.75" thickBot="1">
+    <row r="10" spans="1:20" ht="210.75" hidden="1" thickBot="1">
       <c r="A10" s="20">
         <v>1</v>
       </c>
@@ -4568,7 +4569,7 @@
         <v>44</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>55</v>
@@ -4577,13 +4578,13 @@
         <v>45098</v>
       </c>
       <c r="G10" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="H10" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="H10" s="36" t="s">
+      <c r="I10" s="36" t="s">
         <v>206</v>
-      </c>
-      <c r="I10" s="36" t="s">
-        <v>207</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>76</v>
@@ -4601,7 +4602,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="210.75" thickBot="1">
+    <row r="11" spans="1:20" ht="210.75" hidden="1" thickBot="1">
       <c r="A11" s="20">
         <v>2</v>
       </c>
@@ -4612,7 +4613,7 @@
         <v>44</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>56</v>
@@ -4621,13 +4622,13 @@
         <v>45098</v>
       </c>
       <c r="G11" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="H11" s="36" t="s">
         <v>209</v>
       </c>
-      <c r="H11" s="36" t="s">
+      <c r="I11" s="36" t="s">
         <v>210</v>
-      </c>
-      <c r="I11" s="36" t="s">
-        <v>211</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>76</v>
@@ -4645,7 +4646,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="210.75" thickBot="1">
+    <row r="12" spans="1:20" ht="210.75" hidden="1" thickBot="1">
       <c r="A12" s="20">
         <v>3</v>
       </c>
@@ -4656,7 +4657,7 @@
         <v>44</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E12" s="22" t="s">
         <v>57</v>
@@ -4665,13 +4666,13 @@
         <v>45098</v>
       </c>
       <c r="G12" s="36" t="s">
+        <v>212</v>
+      </c>
+      <c r="H12" s="36" t="s">
         <v>213</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="I12" s="36" t="s">
         <v>214</v>
-      </c>
-      <c r="I12" s="36" t="s">
-        <v>215</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>76</v>
@@ -4689,7 +4690,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="210.75" thickBot="1">
+    <row r="13" spans="1:20" ht="210.75" hidden="1" thickBot="1">
       <c r="A13" s="20">
         <v>4</v>
       </c>
@@ -4700,7 +4701,7 @@
         <v>44</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>58</v>
@@ -4709,13 +4710,13 @@
         <v>45098</v>
       </c>
       <c r="G13" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="H13" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="I13" s="24" t="s">
         <v>219</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>220</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>76</v>
@@ -4733,7 +4734,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="210.75" thickBot="1">
+    <row r="14" spans="1:20" ht="210.75" hidden="1" thickBot="1">
       <c r="A14" s="20">
         <v>5</v>
       </c>
@@ -4744,7 +4745,7 @@
         <v>44</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>59</v>
@@ -4753,13 +4754,13 @@
         <v>45099</v>
       </c>
       <c r="G14" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="H14" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="I14" s="24" t="s">
         <v>223</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>224</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>76</v>
@@ -4777,7 +4778,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="173.25" customHeight="1" thickBot="1">
+    <row r="15" spans="1:20" ht="173.25" hidden="1" customHeight="1" thickBot="1">
       <c r="A15" s="20">
         <v>28</v>
       </c>
@@ -4801,7 +4802,7 @@
         <v>188</v>
       </c>
       <c r="K15" s="54" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>
@@ -4832,35 +4833,35 @@
         <v>72</v>
       </c>
       <c r="F16" s="23">
-        <v>45099</v>
+        <v>45104</v>
       </c>
       <c r="G16" s="36" t="s">
-        <v>225</v>
+        <v>257</v>
       </c>
       <c r="H16" s="36" t="s">
-        <v>226</v>
+        <v>254</v>
       </c>
       <c r="I16" s="24" t="s">
         <v>190</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K16" s="34"/>
       <c r="L16" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="M16" s="54" t="s">
+      <c r="M16" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="N16" s="54" t="s">
-        <v>248</v>
+      <c r="N16" s="34" t="s">
+        <v>255</v>
       </c>
       <c r="O16" s="54" t="s">
         <v>76</v>
       </c>
       <c r="P16" s="33" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="26"/>
@@ -4869,7 +4870,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="105.75" thickBot="1">
+    <row r="17" spans="1:20" ht="105.75" hidden="1" thickBot="1">
       <c r="A17" s="20">
         <v>44</v>
       </c>
@@ -4900,7 +4901,7 @@
       <c r="N17" s="25"/>
       <c r="O17" s="25"/>
       <c r="P17" s="33" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="26"/>
@@ -4909,7 +4910,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="165.75" thickBot="1">
+    <row r="18" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A18" s="20">
         <v>52</v>
       </c>
@@ -4933,7 +4934,7 @@
         <v>188</v>
       </c>
       <c r="K18" s="33" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="L18" s="34"/>
       <c r="M18" s="25"/>
@@ -4947,7 +4948,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="165.75" thickBot="1">
+    <row r="19" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A19" s="20">
         <v>53</v>
       </c>
@@ -4971,7 +4972,7 @@
         <v>188</v>
       </c>
       <c r="K19" s="33" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L19" s="34"/>
       <c r="M19" s="25"/>
@@ -4985,7 +4986,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="165.75" thickBot="1">
+    <row r="20" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A20" s="20">
         <v>54</v>
       </c>
@@ -5009,7 +5010,7 @@
         <v>188</v>
       </c>
       <c r="K20" s="33" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="L20" s="34"/>
       <c r="M20" s="25"/>
@@ -5023,7 +5024,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="165.75" thickBot="1">
+    <row r="21" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A21" s="20">
         <v>55</v>
       </c>
@@ -5047,7 +5048,7 @@
         <v>188</v>
       </c>
       <c r="K21" s="33" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L21" s="34"/>
       <c r="M21" s="25"/>
@@ -5061,7 +5062,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="165.75" thickBot="1">
+    <row r="22" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A22" s="20">
         <v>56</v>
       </c>
@@ -5085,7 +5086,7 @@
         <v>188</v>
       </c>
       <c r="K22" s="33" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="L22" s="34"/>
       <c r="M22" s="25"/>
@@ -5099,7 +5100,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="165.75" thickBot="1">
+    <row r="23" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A23" s="20">
         <v>57</v>
       </c>
@@ -5123,7 +5124,7 @@
         <v>188</v>
       </c>
       <c r="K23" s="33" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="L23" s="34"/>
       <c r="M23" s="25"/>
@@ -5137,7 +5138,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="165.75" thickBot="1">
+    <row r="24" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A24" s="20">
         <v>58</v>
       </c>
@@ -5161,7 +5162,7 @@
         <v>188</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L24" s="34"/>
       <c r="M24" s="25"/>
@@ -5175,7 +5176,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="165.75" thickBot="1">
+    <row r="25" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A25" s="20">
         <v>59</v>
       </c>
@@ -5199,7 +5200,7 @@
         <v>188</v>
       </c>
       <c r="K25" s="33" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="L25" s="34"/>
       <c r="M25" s="25"/>
@@ -5213,7 +5214,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="165.75" thickBot="1">
+    <row r="26" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A26" s="20">
         <v>60</v>
       </c>
@@ -5237,7 +5238,7 @@
         <v>188</v>
       </c>
       <c r="K26" s="33" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="L26" s="34"/>
       <c r="M26" s="25"/>
@@ -5251,7 +5252,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="165.75" thickBot="1">
+    <row r="27" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A27" s="20">
         <v>61</v>
       </c>
@@ -5262,7 +5263,7 @@
         <v>44</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E27" s="22" t="s">
         <v>96</v>
@@ -5271,13 +5272,13 @@
         <v>45099</v>
       </c>
       <c r="G27" s="36" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H27" s="36" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I27" s="36" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="J27" s="33" t="s">
         <v>76</v>
@@ -5290,13 +5291,13 @@
         <v>76</v>
       </c>
       <c r="N27" s="25" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="O27" s="33" t="s">
         <v>76</v>
       </c>
       <c r="P27" s="33" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="26"/>
@@ -5305,7 +5306,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="165.75" thickBot="1">
+    <row r="28" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A28" s="20">
         <v>62</v>
       </c>
@@ -5329,7 +5330,7 @@
         <v>188</v>
       </c>
       <c r="K28" s="33" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="L28" s="34"/>
       <c r="M28" s="25"/>
@@ -5343,7 +5344,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="195.75" thickBot="1">
+    <row r="29" spans="1:20" ht="195.75" hidden="1" thickBot="1">
       <c r="A29" s="40">
         <v>11</v>
       </c>
@@ -5363,13 +5364,13 @@
         <v>45099</v>
       </c>
       <c r="G29" s="36" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H29" s="36" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="I29" s="36" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="J29" s="33" t="s">
         <v>76</v>
@@ -5387,7 +5388,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="195.75" thickBot="1">
+    <row r="30" spans="1:20" ht="195.75" hidden="1" thickBot="1">
       <c r="A30" s="40">
         <v>12</v>
       </c>
@@ -5411,7 +5412,7 @@
         <v>188</v>
       </c>
       <c r="K30" s="33" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="L30" s="34"/>
       <c r="M30" s="33"/>
@@ -5425,7 +5426,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="195.75" thickBot="1">
+    <row r="31" spans="1:20" ht="195.75" hidden="1" thickBot="1">
       <c r="A31" s="40">
         <v>13</v>
       </c>
@@ -5449,7 +5450,7 @@
         <v>188</v>
       </c>
       <c r="K31" s="33" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="L31" s="34"/>
       <c r="M31" s="33"/>
@@ -5463,7 +5464,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="195.75" thickBot="1">
+    <row r="32" spans="1:20" ht="195.75" hidden="1" thickBot="1">
       <c r="A32" s="40">
         <v>14</v>
       </c>
@@ -5487,7 +5488,7 @@
         <v>188</v>
       </c>
       <c r="K32" s="33" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="L32" s="34"/>
       <c r="M32" s="33"/>
@@ -5501,7 +5502,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="210.75" thickBot="1">
+    <row r="33" spans="1:20" ht="210.75" hidden="1" thickBot="1">
       <c r="A33" s="40">
         <v>31</v>
       </c>
@@ -5515,7 +5516,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="39" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F33" s="23"/>
       <c r="G33" s="24"/>
@@ -5525,7 +5526,7 @@
         <v>188</v>
       </c>
       <c r="K33" s="54" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L33" s="34"/>
       <c r="M33" s="34"/>
@@ -5539,7 +5540,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="195.75" thickBot="1">
+    <row r="34" spans="1:20" ht="195">
       <c r="A34" s="40">
         <v>39</v>
       </c>
@@ -5553,38 +5554,38 @@
         <v>73</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F34" s="23">
-        <v>45099</v>
-      </c>
-      <c r="G34" s="24" t="s">
-        <v>191</v>
+        <v>45104</v>
+      </c>
+      <c r="G34" s="36" t="s">
+        <v>258</v>
       </c>
       <c r="H34" s="36" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="I34" s="24" t="s">
         <v>190</v>
       </c>
       <c r="J34" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K34" s="25"/>
-      <c r="L34" s="54" t="s">
+      <c r="L34" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="M34" s="54" t="s">
+      <c r="M34" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="N34" s="54" t="s">
-        <v>248</v>
+      <c r="N34" s="34" t="s">
+        <v>255</v>
       </c>
       <c r="O34" s="54" t="s">
         <v>76</v>
       </c>
       <c r="P34" s="33" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="26"/>
@@ -5593,7 +5594,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="105.75" thickBot="1">
+    <row r="35" spans="1:20" ht="105" hidden="1">
       <c r="A35" s="40">
         <v>47</v>
       </c>
@@ -5624,7 +5625,7 @@
       <c r="N35" s="25"/>
       <c r="O35" s="25"/>
       <c r="P35" s="33" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="Q35" s="25"/>
       <c r="R35" s="26"/>
@@ -5633,7 +5634,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="180.75" thickBot="1">
+    <row r="36" spans="1:20" ht="180" hidden="1">
       <c r="A36" s="40">
         <v>75</v>
       </c>
@@ -5657,7 +5658,7 @@
         <v>188</v>
       </c>
       <c r="K36" s="33" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="L36" s="33"/>
       <c r="M36" s="33"/>
@@ -5671,7 +5672,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="165.75" thickBot="1">
+    <row r="37" spans="1:20" ht="165" hidden="1">
       <c r="A37" s="40">
         <v>76</v>
       </c>
@@ -5695,7 +5696,7 @@
         <v>188</v>
       </c>
       <c r="K37" s="33" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L37" s="33"/>
       <c r="M37" s="33"/>
@@ -5709,7 +5710,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="150.75" thickBot="1">
+    <row r="38" spans="1:20" ht="150" hidden="1">
       <c r="A38" s="40">
         <v>77</v>
       </c>
@@ -5733,7 +5734,7 @@
         <v>188</v>
       </c>
       <c r="K38" s="33" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="L38" s="33"/>
       <c r="M38" s="33"/>
@@ -5747,7 +5748,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="150.75" thickBot="1">
+    <row r="39" spans="1:20" ht="150" hidden="1">
       <c r="A39" s="40">
         <v>78</v>
       </c>
@@ -5771,7 +5772,7 @@
         <v>188</v>
       </c>
       <c r="K39" s="33" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L39" s="33"/>
       <c r="M39" s="33"/>
@@ -5785,7 +5786,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="165.75" thickBot="1">
+    <row r="40" spans="1:20" ht="165" hidden="1">
       <c r="A40" s="40">
         <v>79</v>
       </c>
@@ -5809,7 +5810,7 @@
         <v>188</v>
       </c>
       <c r="K40" s="33" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="L40" s="33"/>
       <c r="M40" s="33"/>
@@ -5823,7 +5824,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="165.75" thickBot="1">
+    <row r="41" spans="1:20" ht="165" hidden="1">
       <c r="A41" s="40">
         <v>80</v>
       </c>
@@ -5847,7 +5848,7 @@
         <v>188</v>
       </c>
       <c r="K41" s="33" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="L41" s="33"/>
       <c r="M41" s="33"/>
@@ -5861,7 +5862,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="165.75" thickBot="1">
+    <row r="42" spans="1:20" ht="165" hidden="1">
       <c r="A42" s="40">
         <v>81</v>
       </c>
@@ -5885,7 +5886,7 @@
         <v>188</v>
       </c>
       <c r="K42" s="33" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="L42" s="25"/>
       <c r="M42" s="25"/>
@@ -5899,7 +5900,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="165.75" thickBot="1">
+    <row r="43" spans="1:20" ht="165" hidden="1">
       <c r="A43" s="40">
         <v>82</v>
       </c>
@@ -5923,7 +5924,7 @@
         <v>188</v>
       </c>
       <c r="K43" s="33" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L43" s="33"/>
       <c r="M43" s="33"/>
@@ -5937,7 +5938,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="150.75" thickBot="1">
+    <row r="44" spans="1:20" ht="150" hidden="1">
       <c r="A44" s="40">
         <v>83</v>
       </c>
@@ -5961,7 +5962,7 @@
         <v>188</v>
       </c>
       <c r="K44" s="33" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="L44" s="33"/>
       <c r="M44" s="33"/>
@@ -5975,7 +5976,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="345.75" thickBot="1">
+    <row r="45" spans="1:20" ht="345.75" hidden="1" thickBot="1">
       <c r="A45" s="40">
         <v>84</v>
       </c>
@@ -5986,7 +5987,7 @@
         <v>48</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E45" s="39" t="s">
         <v>117</v>
@@ -5995,13 +5996,13 @@
         <v>45099</v>
       </c>
       <c r="G45" s="51" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H45" s="55" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="I45" s="56" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="J45" s="47" t="s">
         <v>76</v>
@@ -6014,24 +6015,24 @@
         <v>76</v>
       </c>
       <c r="N45" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O45" s="25" t="s">
         <v>188</v>
       </c>
       <c r="P45" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q45" s="33"/>
       <c r="R45" s="41"/>
       <c r="S45" s="43" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T45" s="42" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="165.75" thickBot="1">
+    <row r="46" spans="1:20" ht="165" hidden="1">
       <c r="A46" s="40">
         <v>85</v>
       </c>
@@ -6055,7 +6056,7 @@
         <v>188</v>
       </c>
       <c r="K46" s="33" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="L46" s="33"/>
       <c r="M46" s="33"/>
@@ -6069,7 +6070,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="165.75" thickBot="1">
+    <row r="47" spans="1:20" ht="165" hidden="1">
       <c r="A47" s="40">
         <v>86</v>
       </c>
@@ -6093,7 +6094,7 @@
         <v>188</v>
       </c>
       <c r="K47" s="33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="L47" s="33"/>
       <c r="M47" s="33"/>
@@ -6107,7 +6108,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="180.75" thickBot="1">
+    <row r="48" spans="1:20" ht="180" hidden="1">
       <c r="A48" s="40">
         <v>87</v>
       </c>
@@ -6131,7 +6132,7 @@
         <v>188</v>
       </c>
       <c r="K48" s="33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="L48" s="33"/>
       <c r="M48" s="33"/>
@@ -6145,7 +6146,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="165.75" thickBot="1">
+    <row r="49" spans="1:20" ht="165" hidden="1">
       <c r="A49" s="40">
         <v>88</v>
       </c>
@@ -6169,7 +6170,7 @@
         <v>188</v>
       </c>
       <c r="K49" s="33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="L49" s="33"/>
       <c r="M49" s="33"/>
@@ -6183,7 +6184,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="150.75" thickBot="1">
+    <row r="50" spans="1:20" ht="150" hidden="1">
       <c r="A50" s="40">
         <v>89</v>
       </c>
@@ -6207,7 +6208,7 @@
         <v>188</v>
       </c>
       <c r="K50" s="33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="L50" s="33"/>
       <c r="M50" s="33"/>
@@ -6221,7 +6222,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="150.75" thickBot="1">
+    <row r="51" spans="1:20" ht="150" hidden="1">
       <c r="A51" s="40">
         <v>90</v>
       </c>
@@ -6245,7 +6246,7 @@
         <v>188</v>
       </c>
       <c r="K51" s="33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="L51" s="33"/>
       <c r="M51" s="33"/>
@@ -6259,7 +6260,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="165.75" thickBot="1">
+    <row r="52" spans="1:20" ht="165" hidden="1">
       <c r="A52" s="40">
         <v>91</v>
       </c>
@@ -6283,7 +6284,7 @@
         <v>188</v>
       </c>
       <c r="K52" s="33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="L52" s="33"/>
       <c r="M52" s="33"/>
@@ -6297,7 +6298,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="165.75" thickBot="1">
+    <row r="53" spans="1:20" ht="165" hidden="1">
       <c r="A53" s="40">
         <v>92</v>
       </c>
@@ -6321,7 +6322,7 @@
         <v>188</v>
       </c>
       <c r="K53" s="33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="L53" s="33"/>
       <c r="M53" s="33"/>
@@ -6335,7 +6336,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="165.75" thickBot="1">
+    <row r="54" spans="1:20" ht="165" hidden="1">
       <c r="A54" s="40">
         <v>93</v>
       </c>
@@ -6359,7 +6360,7 @@
         <v>188</v>
       </c>
       <c r="K54" s="33" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L54" s="33"/>
       <c r="M54" s="33"/>
@@ -6373,7 +6374,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="210">
+    <row r="55" spans="1:20" ht="210" hidden="1">
       <c r="A55" s="20">
         <v>191</v>
       </c>
@@ -6384,10 +6385,10 @@
         <v>44</v>
       </c>
       <c r="D55" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="E55" s="22" t="s">
         <v>199</v>
-      </c>
-      <c r="E55" s="22" t="s">
-        <v>200</v>
       </c>
       <c r="F55" s="23"/>
       <c r="G55" s="24"/>
@@ -6397,7 +6398,7 @@
         <v>188</v>
       </c>
       <c r="K55" s="33" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="L55" s="25"/>
       <c r="M55" s="25"/>
@@ -14869,7 +14870,14 @@
       <c r="T606" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T55" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A9:T55" xr:uid="{00000000-0009-0000-0000-000002000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="36"/>
+        <filter val="39"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -14892,7 +14900,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
D. EVOAggiornamento Test (36,39)
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111AMGMEDICALX/D.EVO/DEVORIS/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111AMGMEDICALX/D.EVO/DEVORIS/1.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progetti\it-fse-accreditamento\GATEWAY\A1#111AMGMEDICALX\D.EVO\DEVORIS\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04001D29-0D44-4F35-AB70-F69A7E66732D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE30E84E-A4F1-42F3-BACB-F8F0CF839C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,9 +432,6 @@
     <t>VALIDAZIONE_TOKEN_JWT_RAD_KO</t>
   </si>
   <si>
-    <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LAB_KO</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -475,9 +472,6 @@
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt avente dei campi valorizzati in maniera errata al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 Al fine di rendere non valido il token è necessario valorizzare il campo "action_id" con la stringa "TEST" (valore non ammesso).</t>
     </r>
-  </si>
-  <si>
-    <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RAD_KO</t>
   </si>
   <si>
     <t>VALIDAZIONE_LAB_TIMEOUT</t>
@@ -1162,19 +1156,25 @@
     <t>Attenzione è obbligatorio valorizzare Il campo "Tipologia Campione"</t>
   </si>
   <si>
-    <t>d2368f4c1c49e9b2</t>
-  </si>
-  <si>
     <t>Campo token JWT non valido, Il campo action_id non è corretto</t>
   </si>
   <si>
-    <t>44ceddc323217c6a</t>
-  </si>
-  <si>
-    <t>2023-06-27T09:38:10Z</t>
-  </si>
-  <si>
-    <t>2023-06-27T09:40:00Z</t>
+    <t>e585819afe60810e</t>
+  </si>
+  <si>
+    <t>2023-06-27T21:51:44Z</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LAB_KO.pdf</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RAD_KO.pdf</t>
+  </si>
+  <si>
+    <t>6697cd85762c3f9d</t>
+  </si>
+  <si>
+    <t>2023-06-27T21:58:45Z</t>
   </si>
 </sst>
 </file>
@@ -2136,8 +2136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4300,8 +4300,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T606"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4316,7 +4316,8 @@
     <col min="8" max="8" width="18.85546875" customWidth="1"/>
     <col min="9" max="9" width="33.140625" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
-    <col min="11" max="15" width="36.42578125" customWidth="1"/>
+    <col min="11" max="11" width="42.5703125" customWidth="1"/>
+    <col min="12" max="15" width="36.42578125" customWidth="1"/>
     <col min="16" max="16" width="27.140625" customWidth="1"/>
     <col min="17" max="17" width="33.140625" customWidth="1"/>
     <col min="18" max="18" width="36.42578125" customWidth="1"/>
@@ -4348,7 +4349,7 @@
       </c>
       <c r="B2" s="60"/>
       <c r="C2" s="61" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D2" s="60"/>
       <c r="F2" s="12"/>
@@ -4373,7 +4374,7 @@
       </c>
       <c r="B3" s="63"/>
       <c r="C3" s="68" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D3" s="69"/>
       <c r="F3" s="12"/>
@@ -4396,7 +4397,7 @@
       <c r="A4" s="64"/>
       <c r="B4" s="65"/>
       <c r="C4" s="70" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D4" s="60"/>
       <c r="E4" s="4"/>
@@ -4420,7 +4421,7 @@
       <c r="A5" s="66"/>
       <c r="B5" s="67"/>
       <c r="C5" s="70" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D5" s="60"/>
       <c r="F5" s="12"/>
@@ -4569,7 +4570,7 @@
         <v>44</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>55</v>
@@ -4578,16 +4579,16 @@
         <v>45098</v>
       </c>
       <c r="G10" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="I10" s="36" t="s">
         <v>204</v>
       </c>
-      <c r="H10" s="36" t="s">
-        <v>205</v>
-      </c>
-      <c r="I10" s="36" t="s">
-        <v>206</v>
-      </c>
       <c r="J10" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K10" s="25"/>
       <c r="L10" s="25"/>
@@ -4613,7 +4614,7 @@
         <v>44</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>56</v>
@@ -4622,16 +4623,16 @@
         <v>45098</v>
       </c>
       <c r="G11" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="H11" s="36" t="s">
+        <v>207</v>
+      </c>
+      <c r="I11" s="36" t="s">
         <v>208</v>
       </c>
-      <c r="H11" s="36" t="s">
-        <v>209</v>
-      </c>
-      <c r="I11" s="36" t="s">
-        <v>210</v>
-      </c>
       <c r="J11" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K11" s="25"/>
       <c r="L11" s="25"/>
@@ -4657,7 +4658,7 @@
         <v>44</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E12" s="22" t="s">
         <v>57</v>
@@ -4666,16 +4667,16 @@
         <v>45098</v>
       </c>
       <c r="G12" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="H12" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="I12" s="36" t="s">
         <v>212</v>
       </c>
-      <c r="H12" s="36" t="s">
-        <v>213</v>
-      </c>
-      <c r="I12" s="36" t="s">
-        <v>214</v>
-      </c>
       <c r="J12" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K12" s="25"/>
       <c r="L12" s="25"/>
@@ -4701,7 +4702,7 @@
         <v>44</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>58</v>
@@ -4710,16 +4711,16 @@
         <v>45098</v>
       </c>
       <c r="G13" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="I13" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="H13" s="24" t="s">
-        <v>218</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>219</v>
-      </c>
       <c r="J13" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K13" s="25"/>
       <c r="L13" s="25"/>
@@ -4745,7 +4746,7 @@
         <v>44</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>59</v>
@@ -4754,16 +4755,16 @@
         <v>45099</v>
       </c>
       <c r="G14" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="I14" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="H14" s="24" t="s">
-        <v>222</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>223</v>
-      </c>
       <c r="J14" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K14" s="25"/>
       <c r="L14" s="25"/>
@@ -4799,10 +4800,10 @@
       <c r="H15" s="24"/>
       <c r="I15" s="24"/>
       <c r="J15" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K15" s="54" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>
@@ -4827,41 +4828,41 @@
         <v>44</v>
       </c>
       <c r="D16" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>71</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>72</v>
       </c>
       <c r="F16" s="23">
         <v>45104</v>
       </c>
       <c r="G16" s="36" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H16" s="36" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K16" s="34"/>
       <c r="L16" s="34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M16" s="34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N16" s="34" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="O16" s="54" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P16" s="33" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="26"/>
@@ -4881,10 +4882,10 @@
         <v>44</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F17" s="23">
         <v>45100</v>
@@ -4893,7 +4894,7 @@
       <c r="H17" s="24"/>
       <c r="I17" s="24"/>
       <c r="J17" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K17" s="25"/>
       <c r="L17" s="34"/>
@@ -4901,7 +4902,7 @@
       <c r="N17" s="25"/>
       <c r="O17" s="25"/>
       <c r="P17" s="33" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="26"/>
@@ -4921,20 +4922,20 @@
         <v>44</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
       <c r="I18" s="24"/>
       <c r="J18" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K18" s="33" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L18" s="34"/>
       <c r="M18" s="25"/>
@@ -4959,20 +4960,20 @@
         <v>44</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
       <c r="J19" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K19" s="33" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="L19" s="34"/>
       <c r="M19" s="25"/>
@@ -4997,20 +4998,20 @@
         <v>44</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F20" s="23"/>
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
       <c r="I20" s="24"/>
       <c r="J20" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K20" s="33" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L20" s="34"/>
       <c r="M20" s="25"/>
@@ -5035,20 +5036,20 @@
         <v>44</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F21" s="23"/>
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
       <c r="I21" s="24"/>
       <c r="J21" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K21" s="33" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L21" s="34"/>
       <c r="M21" s="25"/>
@@ -5073,20 +5074,20 @@
         <v>44</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F22" s="23"/>
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
       <c r="I22" s="24"/>
       <c r="J22" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K22" s="33" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L22" s="34"/>
       <c r="M22" s="25"/>
@@ -5111,20 +5112,20 @@
         <v>44</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F23" s="23"/>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
       <c r="I23" s="24"/>
       <c r="J23" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K23" s="33" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="L23" s="34"/>
       <c r="M23" s="25"/>
@@ -5149,20 +5150,20 @@
         <v>44</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F24" s="23"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
       <c r="I24" s="24"/>
       <c r="J24" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="L24" s="34"/>
       <c r="M24" s="25"/>
@@ -5187,20 +5188,20 @@
         <v>44</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F25" s="23"/>
       <c r="G25" s="24"/>
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
       <c r="J25" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K25" s="33" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="L25" s="34"/>
       <c r="M25" s="25"/>
@@ -5225,20 +5226,20 @@
         <v>44</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F26" s="23"/>
       <c r="G26" s="36"/>
       <c r="H26" s="24"/>
       <c r="I26" s="24"/>
       <c r="J26" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K26" s="33" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="L26" s="34"/>
       <c r="M26" s="25"/>
@@ -5263,41 +5264,41 @@
         <v>44</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F27" s="23">
         <v>45099</v>
       </c>
       <c r="G27" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="H27" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="I27" s="36" t="s">
         <v>235</v>
       </c>
-      <c r="H27" s="36" t="s">
-        <v>236</v>
-      </c>
-      <c r="I27" s="36" t="s">
-        <v>237</v>
-      </c>
       <c r="J27" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K27" s="25"/>
       <c r="L27" s="34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M27" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N27" s="25" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="O27" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P27" s="33" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="26"/>
@@ -5317,20 +5318,20 @@
         <v>44</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F28" s="23"/>
       <c r="G28" s="24"/>
       <c r="H28" s="24"/>
       <c r="I28" s="24"/>
       <c r="J28" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K28" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L28" s="34"/>
       <c r="M28" s="25"/>
@@ -5364,16 +5365,16 @@
         <v>45099</v>
       </c>
       <c r="G29" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="H29" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="I29" s="36" t="s">
         <v>240</v>
       </c>
-      <c r="H29" s="36" t="s">
-        <v>241</v>
-      </c>
-      <c r="I29" s="36" t="s">
-        <v>242</v>
-      </c>
       <c r="J29" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K29" s="33"/>
       <c r="L29" s="34"/>
@@ -5409,10 +5410,10 @@
       <c r="H30" s="36"/>
       <c r="I30" s="36"/>
       <c r="J30" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K30" s="33" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L30" s="34"/>
       <c r="M30" s="33"/>
@@ -5447,10 +5448,10 @@
       <c r="H31" s="36"/>
       <c r="I31" s="36"/>
       <c r="J31" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K31" s="33" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L31" s="34"/>
       <c r="M31" s="33"/>
@@ -5485,10 +5486,10 @@
       <c r="H32" s="36"/>
       <c r="I32" s="36"/>
       <c r="J32" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K32" s="33" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L32" s="34"/>
       <c r="M32" s="33"/>
@@ -5516,17 +5517,17 @@
         <v>70</v>
       </c>
       <c r="E33" s="39" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F33" s="23"/>
       <c r="G33" s="24"/>
       <c r="H33" s="24"/>
       <c r="I33" s="24"/>
       <c r="J33" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K33" s="54" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="L33" s="34"/>
       <c r="M33" s="34"/>
@@ -5551,10 +5552,10 @@
         <v>48</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>73</v>
+        <v>256</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F34" s="23">
         <v>45104</v>
@@ -5563,29 +5564,29 @@
         <v>258</v>
       </c>
       <c r="H34" s="36" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I34" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J34" s="25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K34" s="25"/>
       <c r="L34" s="34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M34" s="34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N34" s="34" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="O34" s="54" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P34" s="33" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="26"/>
@@ -5605,10 +5606,10 @@
         <v>48</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E35" s="39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F35" s="35">
         <v>45099</v>
@@ -5617,7 +5618,7 @@
       <c r="H35" s="24"/>
       <c r="I35" s="24"/>
       <c r="J35" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K35" s="25"/>
       <c r="L35" s="25"/>
@@ -5625,7 +5626,7 @@
       <c r="N35" s="25"/>
       <c r="O35" s="25"/>
       <c r="P35" s="33" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Q35" s="25"/>
       <c r="R35" s="26"/>
@@ -5645,20 +5646,20 @@
         <v>48</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E36" s="39" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F36" s="35"/>
       <c r="G36" s="36"/>
       <c r="H36" s="36"/>
       <c r="I36" s="36"/>
       <c r="J36" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K36" s="33" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L36" s="33"/>
       <c r="M36" s="33"/>
@@ -5683,20 +5684,20 @@
         <v>48</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E37" s="39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F37" s="35"/>
       <c r="G37" s="36"/>
       <c r="H37" s="36"/>
       <c r="I37" s="36"/>
       <c r="J37" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K37" s="33" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="L37" s="33"/>
       <c r="M37" s="33"/>
@@ -5721,20 +5722,20 @@
         <v>48</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E38" s="39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F38" s="35"/>
       <c r="G38" s="36"/>
       <c r="H38" s="36"/>
       <c r="I38" s="36"/>
       <c r="J38" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K38" s="33" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L38" s="33"/>
       <c r="M38" s="33"/>
@@ -5759,20 +5760,20 @@
         <v>48</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E39" s="39" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F39" s="35"/>
       <c r="G39" s="36"/>
       <c r="H39" s="36"/>
       <c r="I39" s="36"/>
       <c r="J39" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K39" s="33" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L39" s="33"/>
       <c r="M39" s="33"/>
@@ -5797,20 +5798,20 @@
         <v>48</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E40" s="39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F40" s="35"/>
       <c r="G40" s="36"/>
       <c r="H40" s="36"/>
       <c r="I40" s="36"/>
       <c r="J40" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K40" s="33" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L40" s="33"/>
       <c r="M40" s="33"/>
@@ -5835,20 +5836,20 @@
         <v>48</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E41" s="39" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F41" s="35"/>
       <c r="G41" s="36"/>
       <c r="H41" s="36"/>
       <c r="I41" s="36"/>
       <c r="J41" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K41" s="33" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="L41" s="33"/>
       <c r="M41" s="33"/>
@@ -5873,20 +5874,20 @@
         <v>48</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E42" s="39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F42" s="35"/>
       <c r="G42" s="36"/>
       <c r="H42" s="36"/>
       <c r="I42" s="36"/>
       <c r="J42" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K42" s="33" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="L42" s="25"/>
       <c r="M42" s="25"/>
@@ -5911,20 +5912,20 @@
         <v>48</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E43" s="39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F43" s="35"/>
       <c r="G43" s="36"/>
       <c r="H43" s="45"/>
       <c r="I43" s="45"/>
       <c r="J43" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K43" s="33" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="L43" s="33"/>
       <c r="M43" s="33"/>
@@ -5949,20 +5950,20 @@
         <v>48</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E44" s="39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F44" s="52"/>
       <c r="G44" s="45"/>
       <c r="H44" s="48"/>
       <c r="I44" s="49"/>
       <c r="J44" s="44" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K44" s="33" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="L44" s="33"/>
       <c r="M44" s="33"/>
@@ -5987,46 +5988,46 @@
         <v>48</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E45" s="39" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F45" s="46">
         <v>45099</v>
       </c>
       <c r="G45" s="51" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H45" s="55" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I45" s="56" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J45" s="47" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K45" s="33"/>
       <c r="L45" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="M45" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N45" s="25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="O45" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="P45" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="Q45" s="33"/>
       <c r="R45" s="41"/>
       <c r="S45" s="43" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="T45" s="42" t="s">
         <v>46</v>
@@ -6043,20 +6044,20 @@
         <v>48</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E46" s="39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F46" s="53"/>
       <c r="G46" s="50"/>
       <c r="H46" s="50"/>
       <c r="I46" s="50"/>
       <c r="J46" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K46" s="33" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="L46" s="33"/>
       <c r="M46" s="33"/>
@@ -6081,20 +6082,20 @@
         <v>48</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E47" s="39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F47" s="35"/>
       <c r="G47" s="36"/>
       <c r="H47" s="36"/>
       <c r="I47" s="36"/>
       <c r="J47" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K47" s="33" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L47" s="33"/>
       <c r="M47" s="33"/>
@@ -6119,20 +6120,20 @@
         <v>48</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E48" s="39" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F48" s="35"/>
       <c r="G48" s="36"/>
       <c r="H48" s="36"/>
       <c r="I48" s="36"/>
       <c r="J48" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K48" s="33" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L48" s="33"/>
       <c r="M48" s="33"/>
@@ -6157,20 +6158,20 @@
         <v>48</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E49" s="39" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F49" s="35"/>
       <c r="G49" s="36"/>
       <c r="H49" s="36"/>
       <c r="I49" s="36"/>
       <c r="J49" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K49" s="33" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L49" s="33"/>
       <c r="M49" s="33"/>
@@ -6195,20 +6196,20 @@
         <v>48</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E50" s="39" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F50" s="35"/>
       <c r="G50" s="36"/>
       <c r="H50" s="36"/>
       <c r="I50" s="36"/>
       <c r="J50" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K50" s="33" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L50" s="33"/>
       <c r="M50" s="33"/>
@@ -6233,20 +6234,20 @@
         <v>48</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E51" s="39" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F51" s="35"/>
       <c r="G51" s="36"/>
       <c r="H51" s="36"/>
       <c r="I51" s="36"/>
       <c r="J51" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K51" s="33" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L51" s="33"/>
       <c r="M51" s="33"/>
@@ -6271,20 +6272,20 @@
         <v>48</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E52" s="39" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F52" s="35"/>
       <c r="G52" s="36"/>
       <c r="H52" s="36"/>
       <c r="I52" s="36"/>
       <c r="J52" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K52" s="33" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L52" s="33"/>
       <c r="M52" s="33"/>
@@ -6309,20 +6310,20 @@
         <v>48</v>
       </c>
       <c r="D53" s="38" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E53" s="39" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F53" s="35"/>
       <c r="G53" s="36"/>
       <c r="H53" s="36"/>
       <c r="I53" s="36"/>
       <c r="J53" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K53" s="33" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L53" s="33"/>
       <c r="M53" s="33"/>
@@ -6347,20 +6348,20 @@
         <v>48</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E54" s="39" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F54" s="35"/>
       <c r="G54" s="36"/>
       <c r="H54" s="36"/>
       <c r="I54" s="36"/>
       <c r="J54" s="33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K54" s="33" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="L54" s="33"/>
       <c r="M54" s="33"/>
@@ -6385,20 +6386,20 @@
         <v>44</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F55" s="23"/>
       <c r="G55" s="24"/>
       <c r="H55" s="24"/>
       <c r="I55" s="24"/>
       <c r="J55" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K55" s="33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L55" s="25"/>
       <c r="M55" s="25"/>
@@ -14922,10 +14923,10 @@
         <v>25</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
@@ -14933,13 +14934,13 @@
         <v>44</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="30" t="s">
         <v>138</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14947,13 +14948,13 @@
         <v>47</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14961,13 +14962,13 @@
         <v>48</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14975,13 +14976,13 @@
         <v>49</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14989,13 +14990,13 @@
         <v>50</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:4" hidden="1">
@@ -15003,13 +15004,13 @@
         <v>51</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:4" hidden="1">
@@ -15017,13 +15018,13 @@
         <v>52</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:4" hidden="1">
@@ -15031,27 +15032,27 @@
         <v>53</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" hidden="1" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C10" s="30">
         <v>191</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1">
@@ -15059,13 +15060,13 @@
         <v>44</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C11" s="30">
         <v>192</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15073,13 +15074,13 @@
         <v>47</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C12" s="30">
         <v>208</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15087,13 +15088,13 @@
         <v>48</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C13" s="30">
         <v>224</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15101,13 +15102,13 @@
         <v>49</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C14" s="30">
         <v>240</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15115,13 +15116,13 @@
         <v>50</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C15" s="30">
         <v>256</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15129,13 +15130,13 @@
         <v>51</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C16" s="30">
         <v>272</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15143,13 +15144,13 @@
         <v>52</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C17" s="30">
         <v>288</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.5" hidden="1" customHeight="1">
@@ -15157,13 +15158,13 @@
         <v>53</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C18" s="30">
         <v>304</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
@@ -15171,13 +15172,13 @@
         <v>44</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C19" s="30">
         <v>193</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15185,13 +15186,13 @@
         <v>47</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C20" s="30">
         <v>209</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15199,13 +15200,13 @@
         <v>48</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C21" s="30">
         <v>225</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15213,13 +15214,13 @@
         <v>49</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C22" s="30">
         <v>241</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15227,13 +15228,13 @@
         <v>50</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C23" s="30">
         <v>257</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15241,13 +15242,13 @@
         <v>51</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C24" s="30">
         <v>273</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15255,13 +15256,13 @@
         <v>52</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C25" s="30">
         <v>289</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15269,13 +15270,13 @@
         <v>53</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C26" s="30">
         <v>305</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
@@ -15283,13 +15284,13 @@
         <v>44</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C27" s="30">
         <v>194</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15297,13 +15298,13 @@
         <v>47</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C28" s="30">
         <v>210</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15311,13 +15312,13 @@
         <v>48</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C29" s="30">
         <v>226</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15325,13 +15326,13 @@
         <v>49</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C30" s="30">
         <v>242</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15339,13 +15340,13 @@
         <v>50</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C31" s="30">
         <v>258</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15353,13 +15354,13 @@
         <v>51</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C32" s="30">
         <v>274</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15367,13 +15368,13 @@
         <v>52</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C33" s="30">
         <v>290</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15381,13 +15382,13 @@
         <v>53</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C34" s="30">
         <v>306</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1">
@@ -15395,7 +15396,7 @@
         <v>44</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C35" s="30">
         <v>195</v>
@@ -15409,7 +15410,7 @@
         <v>47</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C36" s="30">
         <v>211</v>
@@ -15423,7 +15424,7 @@
         <v>48</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C37" s="30">
         <v>227</v>
@@ -15437,7 +15438,7 @@
         <v>49</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C38" s="30">
         <v>243</v>
@@ -15451,7 +15452,7 @@
         <v>50</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C39" s="30">
         <v>259</v>
@@ -15465,7 +15466,7 @@
         <v>51</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C40" s="30">
         <v>275</v>
@@ -15479,7 +15480,7 @@
         <v>52</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C41" s="30">
         <v>291</v>
@@ -15493,7 +15494,7 @@
         <v>53</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C42" s="30">
         <v>307</v>
@@ -15507,7 +15508,7 @@
         <v>44</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C43" s="30">
         <v>196</v>
@@ -15521,7 +15522,7 @@
         <v>47</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C44" s="30">
         <v>212</v>
@@ -15535,7 +15536,7 @@
         <v>48</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C45" s="30">
         <v>228</v>
@@ -15549,7 +15550,7 @@
         <v>49</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C46" s="30">
         <v>244</v>
@@ -15563,7 +15564,7 @@
         <v>50</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C47" s="30">
         <v>260</v>
@@ -15577,7 +15578,7 @@
         <v>51</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C48" s="30">
         <v>276</v>
@@ -15591,7 +15592,7 @@
         <v>52</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C49" s="30">
         <v>292</v>
@@ -15605,7 +15606,7 @@
         <v>53</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C50" s="30">
         <v>308</v>
@@ -16597,18 +16598,18 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
D.EVO Test Ripetuti 29.06.2023
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111AMGMEDICALX/D.EVO/DEVORIS/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111AMGMEDICALX/D.EVO/DEVORIS/1.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progetti\it-fse-accreditamento\GATEWAY\A1#111AMGMEDICALX\D.EVO\DEVORIS\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE30E84E-A4F1-42F3-BACB-F8F0CF839C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDD892B-F7D0-492A-8479-073F0C66F01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -970,21 +970,6 @@
     </r>
   </si>
   <si>
-    <t>2023-04-05T16:45:36Z</t>
-  </si>
-  <si>
-    <t>{
-    "traceID": "73080d6203fbadb5",
-    "spanID": "73080d6203fbadb5",
-    "type": "/msg/syntax",
-    "title": "Errore di sintassi.",
-    "detail": "ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'code' is not valid with respect to its type, 'cs'.",
-    "status": 400,
-    "instance": "/validation/error",
-    "workflowInstanceId": "2.16.840.1.113883.2.9.2.150.4.4.94acb62a90ecf2b5970963e2b6ccecc38052be0abcb8d84f43ef841412b8d449.9fc53d6cd8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"
-}</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_TRASF_CT1</t>
   </si>
   <si>
@@ -1006,66 +991,24 @@
     <t>VAL_CDA2_LAB_CT1</t>
   </si>
   <si>
-    <t>2023-06-21T16:55:43Z</t>
-  </si>
-  <si>
     <t>406809e1ecef64f2</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.3ffb24e356b56193d0bcf074380d1168840605c79d3dd9bc638b11c24a7be892.7d10c045d4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VAL_CDA2_LAB_CT2.pdf</t>
   </si>
   <si>
-    <t>2023-06-21T17:14:37Z</t>
-  </si>
-  <si>
-    <t>1ae755a1f35595fe</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.64c3ac8ab189f59c8d8a1d9e8adc6109d43b384a9d5f5266bee0b684196a19eb.99664107aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VAL_CDA2_LAB_CT3.pdf</t>
   </si>
   <si>
-    <t>2023-06-21T17:33:24Z</t>
-  </si>
-  <si>
-    <t>5620bbcc68bbe91c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.aa7cb8dd13f61c5aaee7421cbbe3c22d0d3e8e2c100245479d1f079532e8df0a.e35842f497^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Il software vincola la compilazione dei campi obbligatori per la generazione del token JWT</t>
   </si>
   <si>
     <t>VAL_CDA2_LAB_CT4.pdf</t>
   </si>
   <si>
-    <t>2023-06-21T21:44:32Z</t>
-  </si>
-  <si>
-    <t>6e9ee617e6f32fbb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.d83f8d332413d65de0d94cfa8e309aa82c51ea2ce2d674bc297644f957471d8d.e09468be85^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VAL_CDA2_LAB_CT5.pdf</t>
   </si>
   <si>
-    <t>2023-06-22T11:42:42Z</t>
-  </si>
-  <si>
-    <t>8b16d1dce95478d6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.aa7cb8dd13f61c5aaee7421cbbe3c22d0d3e8e2c100245479d1f079532e8df0a.e0c74447c9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">Viene mostrato a video il messaggio di errore "TIME OUT VALIDAZIONE". Il medico può produrre il referto e l'invio al FSE rimarrà in coda fino al ripristino del servizio. </t>
   </si>
   <si>
@@ -1099,30 +1042,12 @@
     <t>VAL_CDA2_LAB_CT15_KO</t>
   </si>
   <si>
-    <t>2023-06-22T13:06:00Z</t>
-  </si>
-  <si>
-    <t>fa9aee7d55f4b57b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.3b4dfbfa8a55d2aa3e03d86a951b7089defbd67c58e77c3504b6134fb73b597f.4d04954f20^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Si rende necessaria la correzione della configurazione dell'esame, il referto deve essere riprodotto</t>
   </si>
   <si>
     <t>L'elemento è obbligatorio per la generazione del REFERTO CDA2</t>
   </si>
   <si>
-    <t>2023-06-22T13:40:30Z</t>
-  </si>
-  <si>
-    <t>ce640d091bdf7ddd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.42f0d4e3c3a8f48f5f8ca73180331bc6ba7ed86bec3913f34b732951b8ef4496.a57b650eb2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Il Software non gestisce le sezioni opzionali</t>
   </si>
   <si>
@@ -1132,12 +1057,6 @@
     <t>Il software vincola la compilazione dei soli codici associati al dizionario "ISCO-08"</t>
   </si>
   <si>
-    <t>e1363f989485bda5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.42f0d4e3c3a8f48f5f8ca73180331bc6ba7ed86bec3913f34b732951b8ef4496.8604237bf0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VAL_CDA2_RAD_CT14_KO</t>
   </si>
   <si>
@@ -1159,29 +1078,101 @@
     <t>Campo token JWT non valido, Il campo action_id non è corretto</t>
   </si>
   <si>
-    <t>e585819afe60810e</t>
-  </si>
-  <si>
-    <t>2023-06-27T21:51:44Z</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LAB_KO.pdf</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RAD_KO.pdf</t>
   </si>
   <si>
-    <t>6697cd85762c3f9d</t>
-  </si>
-  <si>
-    <t>2023-06-27T21:58:45Z</t>
+    <t>2023-06-29T09:47:07Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.3ffb24e356b56193d0bcf074380d1168840605c79d3dd9bc638b11c24a7be892.3a9d0a9c7f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>513e6219621f57d8</t>
+  </si>
+  <si>
+    <t>2023-06-29T09:50:54Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.64c3ac8ab189f59c8d8a1d9e8adc6109d43b384a9d5f5266bee0b684196a19eb.b30aff384b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.aa7cb8dd13f61c5aaee7421cbbe3c22d0d3e8e2c100245479d1f079532e8df0a.9741eda083^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-29T09:53:20Z</t>
+  </si>
+  <si>
+    <t>acb769f2144dbf9f</t>
+  </si>
+  <si>
+    <t>2023-06-29T10:04:29Z</t>
+  </si>
+  <si>
+    <t>bbd5a28900bb36da</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.d83f8d332413d65de0d94cfa8e309aa82c51ea2ce2d674bc297644f957471d8d.2502a54a06^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-29T10:08:29Z</t>
+  </si>
+  <si>
+    <t>3e5df3efd6322f37</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.aa7cb8dd13f61c5aaee7421cbbe3c22d0d3e8e2c100245479d1f079532e8df0a.aad95cdb7e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-29T10:10:42Z</t>
+  </si>
+  <si>
+    <t>d6400394041041f7</t>
+  </si>
+  <si>
+    <t>2023-06-29T10:12:15Z</t>
+  </si>
+  <si>
+    <t>3f8d90eeb9a1239e</t>
+  </si>
+  <si>
+    <t>2023-06-29T10:14:23Z</t>
+  </si>
+  <si>
+    <t>41eb60925230e8e3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.3b4dfbfa8a55d2aa3e03d86a951b7089defbd67c58e77c3504b6134fb73b597f.a2256281a4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-29T10:26:23Z</t>
+  </si>
+  <si>
+    <t>f05bd696d13b9843</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.42f0d4e3c3a8f48f5f8ca73180331bc6ba7ed86bec3913f34b732951b8ef4496.9d0c147a81^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4518d74cc8bfe400</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.42f0d4e3c3a8f48f5f8ca73180331bc6ba7ed86bec3913f34b732951b8ef4496.8e233b0914^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-29T10:29:44Z</t>
+  </si>
+  <si>
+    <t>{"traceID":"4518d74cc8bfe400","spanID":"4518d74cc8bfe400","type":"/msg/syntax","title":"Errore di sintassi.","detail":"ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'code' is not valid with respect to its type, 'cs'.","status":400,"instance":"/validation/error","workflowInstanceId":"2.16.840.1.113883.2.9.2.150.4.4.42f0d4e3c3a8f48f5f8ca73180331bc6ba7ed86bec3913f34b732951b8ef4496.8e233b0914^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1276,6 +1267,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1653,7 +1651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1797,9 +1795,6 @@
     <xf numFmtId="14" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="14" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1808,12 +1803,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1840,6 +1829,24 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4300,8 +4307,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T606"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S56" sqref="S56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4344,14 +4351,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="61" t="s">
-        <v>200</v>
-      </c>
-      <c r="D2" s="60"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="57"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -4369,14 +4376,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="68" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" s="69"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" s="66"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -4394,12 +4401,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="70" t="s">
-        <v>199</v>
-      </c>
-      <c r="D4" s="60"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="67" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" s="57"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -4418,12 +4425,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+      <c r="A5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="67" t="s">
         <v>187</v>
       </c>
-      <c r="D5" s="60"/>
+      <c r="D5" s="57"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4441,8 +4448,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="57"/>
-      <c r="B6" s="58"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="55"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4559,7 +4566,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="210.75" hidden="1" thickBot="1">
+    <row r="10" spans="1:20" ht="210.75" thickBot="1">
       <c r="A10" s="20">
         <v>1</v>
       </c>
@@ -4570,22 +4577,22 @@
         <v>44</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>55</v>
       </c>
       <c r="F10" s="23">
-        <v>45098</v>
+        <v>45106</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I10" s="36" t="s">
-        <v>204</v>
+        <v>232</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>74</v>
@@ -4603,7 +4610,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="210.75" hidden="1" thickBot="1">
+    <row r="11" spans="1:20" ht="210.75" thickBot="1">
       <c r="A11" s="20">
         <v>2</v>
       </c>
@@ -4614,22 +4621,22 @@
         <v>44</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>56</v>
       </c>
       <c r="F11" s="23">
-        <v>45098</v>
+        <v>45106</v>
       </c>
       <c r="G11" s="36" t="s">
-        <v>206</v>
-      </c>
-      <c r="H11" s="36" t="s">
-        <v>207</v>
+        <v>234</v>
+      </c>
+      <c r="H11" s="68" t="s">
+        <v>233</v>
       </c>
       <c r="I11" s="36" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>74</v>
@@ -4647,7 +4654,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="210.75" hidden="1" thickBot="1">
+    <row r="12" spans="1:20" ht="210.75" thickBot="1">
       <c r="A12" s="20">
         <v>3</v>
       </c>
@@ -4658,22 +4665,22 @@
         <v>44</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="E12" s="22" t="s">
         <v>57</v>
       </c>
       <c r="F12" s="23">
-        <v>45098</v>
+        <v>45106</v>
       </c>
       <c r="G12" s="36" t="s">
-        <v>210</v>
+        <v>237</v>
       </c>
       <c r="H12" s="36" t="s">
-        <v>211</v>
+        <v>238</v>
       </c>
       <c r="I12" s="36" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>74</v>
@@ -4691,7 +4698,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="210.75" hidden="1" thickBot="1">
+    <row r="13" spans="1:20" ht="210.75" thickBot="1">
       <c r="A13" s="20">
         <v>4</v>
       </c>
@@ -4702,22 +4709,22 @@
         <v>44</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>58</v>
       </c>
       <c r="F13" s="23">
-        <v>45098</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>215</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>217</v>
+        <v>45106</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="H13" s="36" t="s">
+        <v>240</v>
+      </c>
+      <c r="I13" s="36" t="s">
+        <v>241</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>74</v>
@@ -4735,7 +4742,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="210.75" hidden="1" thickBot="1">
+    <row r="14" spans="1:20" ht="210.75" thickBot="1">
       <c r="A14" s="20">
         <v>5</v>
       </c>
@@ -4746,22 +4753,22 @@
         <v>44</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="23">
-        <v>45099</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>220</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>221</v>
+      <c r="F14" s="70">
+        <v>45106</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="H14" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="I14" s="36" t="s">
+        <v>244</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>74</v>
@@ -4802,8 +4809,8 @@
       <c r="J15" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="K15" s="54" t="s">
-        <v>213</v>
+      <c r="K15" s="53" t="s">
+        <v>203</v>
       </c>
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>
@@ -4828,19 +4835,19 @@
         <v>44</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="E16" s="22" t="s">
         <v>71</v>
       </c>
       <c r="F16" s="23">
-        <v>45104</v>
+        <v>45106</v>
       </c>
       <c r="G16" s="36" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="H16" s="36" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="I16" s="24" t="s">
         <v>188</v>
@@ -4856,13 +4863,13 @@
         <v>74</v>
       </c>
       <c r="N16" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="O16" s="54" t="s">
+        <v>228</v>
+      </c>
+      <c r="O16" s="53" t="s">
         <v>74</v>
       </c>
       <c r="P16" s="33" t="s">
-        <v>242</v>
+        <v>220</v>
       </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="26"/>
@@ -4902,7 +4909,7 @@
       <c r="N17" s="25"/>
       <c r="O17" s="25"/>
       <c r="P17" s="33" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="26"/>
@@ -4935,7 +4942,7 @@
         <v>186</v>
       </c>
       <c r="K18" s="33" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="L18" s="34"/>
       <c r="M18" s="25"/>
@@ -4973,7 +4980,7 @@
         <v>186</v>
       </c>
       <c r="K19" s="33" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="L19" s="34"/>
       <c r="M19" s="25"/>
@@ -5011,7 +5018,7 @@
         <v>186</v>
       </c>
       <c r="K20" s="33" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="L20" s="34"/>
       <c r="M20" s="25"/>
@@ -5049,7 +5056,7 @@
         <v>186</v>
       </c>
       <c r="K21" s="33" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="L21" s="34"/>
       <c r="M21" s="25"/>
@@ -5087,7 +5094,7 @@
         <v>186</v>
       </c>
       <c r="K22" s="33" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="L22" s="34"/>
       <c r="M22" s="25"/>
@@ -5125,7 +5132,7 @@
         <v>186</v>
       </c>
       <c r="K23" s="33" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="L23" s="34"/>
       <c r="M23" s="25"/>
@@ -5163,7 +5170,7 @@
         <v>186</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="L24" s="34"/>
       <c r="M24" s="25"/>
@@ -5201,7 +5208,7 @@
         <v>186</v>
       </c>
       <c r="K25" s="33" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="L25" s="34"/>
       <c r="M25" s="25"/>
@@ -5239,7 +5246,7 @@
         <v>186</v>
       </c>
       <c r="K26" s="33" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="L26" s="34"/>
       <c r="M26" s="25"/>
@@ -5253,7 +5260,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="27" spans="1:20" ht="165.75" thickBot="1">
       <c r="A27" s="20">
         <v>61</v>
       </c>
@@ -5264,22 +5271,22 @@
         <v>44</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="E27" s="22" t="s">
         <v>94</v>
       </c>
       <c r="F27" s="23">
-        <v>45099</v>
+        <v>45106</v>
       </c>
       <c r="G27" s="36" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="H27" s="36" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="I27" s="36" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="J27" s="33" t="s">
         <v>74</v>
@@ -5292,13 +5299,13 @@
         <v>74</v>
       </c>
       <c r="N27" s="25" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="O27" s="33" t="s">
         <v>74</v>
       </c>
       <c r="P27" s="33" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="26"/>
@@ -5331,7 +5338,7 @@
         <v>186</v>
       </c>
       <c r="K28" s="33" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="L28" s="34"/>
       <c r="M28" s="25"/>
@@ -5345,7 +5352,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="195.75" hidden="1" thickBot="1">
+    <row r="29" spans="1:20" ht="195.75" thickBot="1">
       <c r="A29" s="40">
         <v>11</v>
       </c>
@@ -5362,16 +5369,16 @@
         <v>61</v>
       </c>
       <c r="F29" s="35">
-        <v>45099</v>
+        <v>45106</v>
       </c>
       <c r="G29" s="36" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="H29" s="36" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="I29" s="36" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="J29" s="33" t="s">
         <v>74</v>
@@ -5413,7 +5420,7 @@
         <v>186</v>
       </c>
       <c r="K30" s="33" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="L30" s="34"/>
       <c r="M30" s="33"/>
@@ -5451,7 +5458,7 @@
         <v>186</v>
       </c>
       <c r="K31" s="33" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="L31" s="34"/>
       <c r="M31" s="33"/>
@@ -5489,7 +5496,7 @@
         <v>186</v>
       </c>
       <c r="K32" s="33" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="L32" s="34"/>
       <c r="M32" s="33"/>
@@ -5526,8 +5533,8 @@
       <c r="J33" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="K33" s="54" t="s">
-        <v>213</v>
+      <c r="K33" s="53" t="s">
+        <v>203</v>
       </c>
       <c r="L33" s="34"/>
       <c r="M33" s="34"/>
@@ -5541,7 +5548,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="195">
+    <row r="34" spans="1:20" ht="195.75" thickBot="1">
       <c r="A34" s="40">
         <v>39</v>
       </c>
@@ -5552,19 +5559,19 @@
         <v>48</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="E34" s="39" t="s">
         <v>193</v>
       </c>
       <c r="F34" s="23">
-        <v>45104</v>
+        <v>45106</v>
       </c>
       <c r="G34" s="36" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="H34" s="36" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="I34" s="24" t="s">
         <v>188</v>
@@ -5580,13 +5587,13 @@
         <v>74</v>
       </c>
       <c r="N34" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="O34" s="54" t="s">
+        <v>228</v>
+      </c>
+      <c r="O34" s="53" t="s">
         <v>74</v>
       </c>
       <c r="P34" s="33" t="s">
-        <v>242</v>
+        <v>220</v>
       </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="26"/>
@@ -5595,7 +5602,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="105" hidden="1">
+    <row r="35" spans="1:20" ht="105.75" hidden="1" thickBot="1">
       <c r="A35" s="40">
         <v>47</v>
       </c>
@@ -5626,7 +5633,7 @@
       <c r="N35" s="25"/>
       <c r="O35" s="25"/>
       <c r="P35" s="33" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="Q35" s="25"/>
       <c r="R35" s="26"/>
@@ -5635,7 +5642,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="180" hidden="1">
+    <row r="36" spans="1:20" ht="180.75" hidden="1" thickBot="1">
       <c r="A36" s="40">
         <v>75</v>
       </c>
@@ -5659,7 +5666,7 @@
         <v>186</v>
       </c>
       <c r="K36" s="33" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="L36" s="33"/>
       <c r="M36" s="33"/>
@@ -5673,7 +5680,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="165" hidden="1">
+    <row r="37" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A37" s="40">
         <v>76</v>
       </c>
@@ -5697,7 +5704,7 @@
         <v>186</v>
       </c>
       <c r="K37" s="33" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="L37" s="33"/>
       <c r="M37" s="33"/>
@@ -5711,7 +5718,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="150" hidden="1">
+    <row r="38" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A38" s="40">
         <v>77</v>
       </c>
@@ -5735,7 +5742,7 @@
         <v>186</v>
       </c>
       <c r="K38" s="33" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="L38" s="33"/>
       <c r="M38" s="33"/>
@@ -5749,7 +5756,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="150" hidden="1">
+    <row r="39" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A39" s="40">
         <v>78</v>
       </c>
@@ -5773,7 +5780,7 @@
         <v>186</v>
       </c>
       <c r="K39" s="33" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="L39" s="33"/>
       <c r="M39" s="33"/>
@@ -5787,7 +5794,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="165" hidden="1">
+    <row r="40" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A40" s="40">
         <v>79</v>
       </c>
@@ -5811,7 +5818,7 @@
         <v>186</v>
       </c>
       <c r="K40" s="33" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="L40" s="33"/>
       <c r="M40" s="33"/>
@@ -5825,7 +5832,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="165" hidden="1">
+    <row r="41" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A41" s="40">
         <v>80</v>
       </c>
@@ -5849,7 +5856,7 @@
         <v>186</v>
       </c>
       <c r="K41" s="33" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="L41" s="33"/>
       <c r="M41" s="33"/>
@@ -5863,7 +5870,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="165" hidden="1">
+    <row r="42" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A42" s="40">
         <v>81</v>
       </c>
@@ -5887,7 +5894,7 @@
         <v>186</v>
       </c>
       <c r="K42" s="33" t="s">
-        <v>243</v>
+        <v>221</v>
       </c>
       <c r="L42" s="25"/>
       <c r="M42" s="25"/>
@@ -5901,7 +5908,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="165" hidden="1">
+    <row r="43" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A43" s="40">
         <v>82</v>
       </c>
@@ -5925,7 +5932,7 @@
         <v>186</v>
       </c>
       <c r="K43" s="33" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="L43" s="33"/>
       <c r="M43" s="33"/>
@@ -5939,7 +5946,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="150" hidden="1">
+    <row r="44" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A44" s="40">
         <v>83</v>
       </c>
@@ -5955,7 +5962,7 @@
       <c r="E44" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F44" s="52"/>
+      <c r="F44" s="51"/>
       <c r="G44" s="45"/>
       <c r="H44" s="48"/>
       <c r="I44" s="49"/>
@@ -5963,7 +5970,7 @@
         <v>186</v>
       </c>
       <c r="K44" s="33" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="L44" s="33"/>
       <c r="M44" s="33"/>
@@ -5977,7 +5984,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="345.75" hidden="1" thickBot="1">
+    <row r="45" spans="1:20" ht="270.75" thickBot="1">
       <c r="A45" s="40">
         <v>84</v>
       </c>
@@ -5988,22 +5995,22 @@
         <v>48</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="E45" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F45" s="46">
-        <v>45099</v>
-      </c>
-      <c r="G45" s="51" t="s">
-        <v>194</v>
-      </c>
-      <c r="H45" s="55" t="s">
-        <v>244</v>
-      </c>
-      <c r="I45" s="56" t="s">
-        <v>245</v>
+        <v>45106</v>
+      </c>
+      <c r="G45" s="46" t="s">
+        <v>257</v>
+      </c>
+      <c r="H45" s="72" t="s">
+        <v>255</v>
+      </c>
+      <c r="I45" s="73" t="s">
+        <v>256</v>
       </c>
       <c r="J45" s="47" t="s">
         <v>74</v>
@@ -6027,7 +6034,7 @@
       <c r="Q45" s="33"/>
       <c r="R45" s="41"/>
       <c r="S45" s="43" t="s">
-        <v>195</v>
+        <v>258</v>
       </c>
       <c r="T45" s="42" t="s">
         <v>46</v>
@@ -6049,7 +6056,7 @@
       <c r="E46" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="F46" s="53"/>
+      <c r="F46" s="52"/>
       <c r="G46" s="50"/>
       <c r="H46" s="50"/>
       <c r="I46" s="50"/>
@@ -6057,7 +6064,7 @@
         <v>186</v>
       </c>
       <c r="K46" s="33" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="L46" s="33"/>
       <c r="M46" s="33"/>
@@ -6095,7 +6102,7 @@
         <v>186</v>
       </c>
       <c r="K47" s="33" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="L47" s="33"/>
       <c r="M47" s="33"/>
@@ -6133,7 +6140,7 @@
         <v>186</v>
       </c>
       <c r="K48" s="33" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="L48" s="33"/>
       <c r="M48" s="33"/>
@@ -6171,7 +6178,7 @@
         <v>186</v>
       </c>
       <c r="K49" s="33" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="L49" s="33"/>
       <c r="M49" s="33"/>
@@ -6209,7 +6216,7 @@
         <v>186</v>
       </c>
       <c r="K50" s="33" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="L50" s="33"/>
       <c r="M50" s="33"/>
@@ -6247,7 +6254,7 @@
         <v>186</v>
       </c>
       <c r="K51" s="33" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="L51" s="33"/>
       <c r="M51" s="33"/>
@@ -6285,7 +6292,7 @@
         <v>186</v>
       </c>
       <c r="K52" s="33" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="L52" s="33"/>
       <c r="M52" s="33"/>
@@ -6323,7 +6330,7 @@
         <v>186</v>
       </c>
       <c r="K53" s="33" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="L53" s="33"/>
       <c r="M53" s="33"/>
@@ -6361,7 +6368,7 @@
         <v>186</v>
       </c>
       <c r="K54" s="33" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="L54" s="33"/>
       <c r="M54" s="33"/>
@@ -6386,10 +6393,10 @@
         <v>44</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F55" s="23"/>
       <c r="G55" s="24"/>
@@ -6399,7 +6406,7 @@
         <v>186</v>
       </c>
       <c r="K55" s="33" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="L55" s="25"/>
       <c r="M55" s="25"/>
@@ -6414,10 +6421,10 @@
       </c>
     </row>
     <row r="56" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F56" s="12"/>
+      <c r="F56" s="69"/>
       <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
+      <c r="H56" s="71"/>
+      <c r="I56" s="69"/>
       <c r="J56" s="13"/>
       <c r="K56" s="13"/>
       <c r="L56" s="13"/>
@@ -14872,10 +14879,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:T55" xr:uid="{00000000-0009-0000-0000-000002000000}">
-    <filterColumn colId="0">
+    <filterColumn colId="5">
       <filters>
-        <filter val="36"/>
-        <filter val="39"/>
+        <dateGroupItem year="2023" month="6" day="29" dateTimeGrouping="day"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
D.EVO Ripetizione test (30.06.2023)
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111AMGMEDICALX/D.EVO/DEVORIS/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111AMGMEDICALX/D.EVO/DEVORIS/1.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progetti\it-fse-accreditamento\GATEWAY\A1#111AMGMEDICALX\D.EVO\DEVORIS\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDD892B-F7D0-492A-8479-073F0C66F01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0C4235-9C2D-4EB1-8DDF-76DF673851B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -991,9 +991,6 @@
     <t>VAL_CDA2_LAB_CT1</t>
   </si>
   <si>
-    <t>406809e1ecef64f2</t>
-  </si>
-  <si>
     <t>VAL_CDA2_LAB_CT2.pdf</t>
   </si>
   <si>
@@ -1084,88 +1081,91 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RAD_KO.pdf</t>
   </si>
   <si>
-    <t>2023-06-29T09:47:07Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.3ffb24e356b56193d0bcf074380d1168840605c79d3dd9bc638b11c24a7be892.3a9d0a9c7f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>513e6219621f57d8</t>
-  </si>
-  <si>
-    <t>2023-06-29T09:50:54Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.64c3ac8ab189f59c8d8a1d9e8adc6109d43b384a9d5f5266bee0b684196a19eb.b30aff384b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.aa7cb8dd13f61c5aaee7421cbbe3c22d0d3e8e2c100245479d1f079532e8df0a.9741eda083^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-06-29T09:53:20Z</t>
-  </si>
-  <si>
-    <t>acb769f2144dbf9f</t>
-  </si>
-  <si>
-    <t>2023-06-29T10:04:29Z</t>
-  </si>
-  <si>
-    <t>bbd5a28900bb36da</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.d83f8d332413d65de0d94cfa8e309aa82c51ea2ce2d674bc297644f957471d8d.2502a54a06^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-06-29T10:08:29Z</t>
-  </si>
-  <si>
-    <t>3e5df3efd6322f37</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.aa7cb8dd13f61c5aaee7421cbbe3c22d0d3e8e2c100245479d1f079532e8df0a.aad95cdb7e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-06-29T10:10:42Z</t>
-  </si>
-  <si>
-    <t>d6400394041041f7</t>
-  </si>
-  <si>
-    <t>2023-06-29T10:12:15Z</t>
-  </si>
-  <si>
-    <t>3f8d90eeb9a1239e</t>
-  </si>
-  <si>
-    <t>2023-06-29T10:14:23Z</t>
-  </si>
-  <si>
     <t>41eb60925230e8e3</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.3b4dfbfa8a55d2aa3e03d86a951b7089defbd67c58e77c3504b6134fb73b597f.a2256281a4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-06-29T10:26:23Z</t>
-  </si>
-  <si>
-    <t>f05bd696d13b9843</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.42f0d4e3c3a8f48f5f8ca73180331bc6ba7ed86bec3913f34b732951b8ef4496.9d0c147a81^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>4518d74cc8bfe400</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.42f0d4e3c3a8f48f5f8ca73180331bc6ba7ed86bec3913f34b732951b8ef4496.8e233b0914^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-06-29T10:29:44Z</t>
-  </si>
-  <si>
-    <t>{"traceID":"4518d74cc8bfe400","spanID":"4518d74cc8bfe400","type":"/msg/syntax","title":"Errore di sintassi.","detail":"ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'code' is not valid with respect to its type, 'cs'.","status":400,"instance":"/validation/error","workflowInstanceId":"2.16.840.1.113883.2.9.2.150.4.4.42f0d4e3c3a8f48f5f8ca73180331bc6ba7ed86bec3913f34b732951b8ef4496.8e233b0914^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"}</t>
+    <t>889134a83e323be5</t>
+  </si>
+  <si>
+    <t>2023-06-30T17:12:08Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.3ffb24e356b56193d0bcf074380d1168840605c79d3dd9bc638b11c24a7be892.fa12f3637d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-30T17:14:45Z</t>
+  </si>
+  <si>
+    <t>7fee733315009e6a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.64c3ac8ab189f59c8d8a1d9e8adc6109d43b384a9d5f5266bee0b684196a19eb.673791290b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f9b9b7d4ede84b99</t>
+  </si>
+  <si>
+    <t>2023-06-30T17:16:23Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.aa7cb8dd13f61c5aaee7421cbbe3c22d0d3e8e2c100245479d1f079532e8df0a.8d64173328^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-30T17:18:12Z</t>
+  </si>
+  <si>
+    <t>63a839e0bb80b954</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.d83f8d332413d65de0d94cfa8e309aa82c51ea2ce2d674bc297644f957471d8d.501be55616^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-30T17:19:30Z</t>
+  </si>
+  <si>
+    <t>bdcf130bd1970a20</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.aa7cb8dd13f61c5aaee7421cbbe3c22d0d3e8e2c100245479d1f079532e8df0a.dccd89da32^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-30T17:22:59Z</t>
+  </si>
+  <si>
+    <t>dbfda070267d5d41</t>
+  </si>
+  <si>
+    <t>2023-06-30T17:24:49Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.3b4dfbfa8a55d2aa3e03d86a951b7089defbd67c58e77c3504b6134fb73b597f.d3436fd82f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-30T17:27:34Z</t>
+  </si>
+  <si>
+    <t>a90209001a90a9f5</t>
+  </si>
+  <si>
+    <t>2023-06-30T17:29:10Z</t>
+  </si>
+  <si>
+    <t>ab53552883bb72a2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.42f0d4e3c3a8f48f5f8ca73180331bc6ba7ed86bec3913f34b732951b8ef4496.e21db04bc4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-30T17:30:46Z</t>
+  </si>
+  <si>
+    <t>1a8015f8831984b9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.42f0d4e3c3a8f48f5f8ca73180331bc6ba7ed86bec3913f34b732951b8ef4496.4a632a3010^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>{"traceID":"1a8015f8831984b9","spanID":"1a8015f8831984b9","type":"/msg/syntax","title":"Errore di sintassi.","detail":"ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'code' is not valid with respect to its type, 'cs'.","status":400,"instance":"/validation/error","workflowInstanceId":"2.16.840.1.113883.2.9.2.150.4.4.42f0d4e3c3a8f48f5f8ca73180331bc6ba7ed86bec3913f34b732951b8ef4496.4a632a3010^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"}</t>
   </si>
 </sst>
 </file>
@@ -1298,7 +1298,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1609,19 +1609,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -1651,7 +1638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1795,14 +1782,23 @@
     <xf numFmtId="14" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1830,22 +1826,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4304,11 +4285,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:T606"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S56" sqref="S56"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4351,14 +4331,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58" t="s">
+      <c r="B2" s="60"/>
+      <c r="C2" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="D2" s="57"/>
+      <c r="D2" s="60"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -4376,14 +4356,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="65" t="s">
+      <c r="B3" s="63"/>
+      <c r="C3" s="68" t="s">
         <v>196</v>
       </c>
-      <c r="D3" s="66"/>
+      <c r="D3" s="69"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -4401,12 +4381,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="61"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="67" t="s">
+      <c r="A4" s="64"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="70" t="s">
         <v>197</v>
       </c>
-      <c r="D4" s="57"/>
+      <c r="D4" s="60"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -4425,12 +4405,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="63"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>187</v>
       </c>
-      <c r="D5" s="57"/>
+      <c r="D5" s="60"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4448,8 +4428,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4583,16 +4563,16 @@
         <v>55</v>
       </c>
       <c r="F10" s="23">
-        <v>45106</v>
+        <v>45107</v>
       </c>
       <c r="G10" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="H10" s="36" t="s">
         <v>231</v>
       </c>
-      <c r="H10" s="36" t="s">
-        <v>200</v>
-      </c>
       <c r="I10" s="36" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>74</v>
@@ -4621,22 +4601,22 @@
         <v>44</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>56</v>
       </c>
       <c r="F11" s="23">
-        <v>45106</v>
+        <v>45107</v>
       </c>
       <c r="G11" s="36" t="s">
         <v>234</v>
       </c>
-      <c r="H11" s="68" t="s">
-        <v>233</v>
+      <c r="H11" s="54" t="s">
+        <v>235</v>
       </c>
       <c r="I11" s="36" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>74</v>
@@ -4665,22 +4645,22 @@
         <v>44</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E12" s="22" t="s">
         <v>57</v>
       </c>
       <c r="F12" s="23">
-        <v>45106</v>
+        <v>45107</v>
       </c>
       <c r="G12" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="H12" s="36" t="s">
         <v>237</v>
       </c>
-      <c r="H12" s="36" t="s">
-        <v>238</v>
-      </c>
       <c r="I12" s="36" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>74</v>
@@ -4709,22 +4689,22 @@
         <v>44</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>58</v>
       </c>
       <c r="F13" s="23">
-        <v>45106</v>
+        <v>45107</v>
       </c>
       <c r="G13" s="36" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H13" s="36" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I13" s="36" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>74</v>
@@ -4753,22 +4733,22 @@
         <v>44</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="70">
-        <v>45106</v>
+      <c r="F14" s="56">
+        <v>45107</v>
       </c>
       <c r="G14" s="36" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H14" s="36" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I14" s="36" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>74</v>
@@ -4786,7 +4766,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="173.25" hidden="1" customHeight="1" thickBot="1">
+    <row r="15" spans="1:20" ht="173.25" customHeight="1" thickBot="1">
       <c r="A15" s="20">
         <v>28</v>
       </c>
@@ -4810,7 +4790,7 @@
         <v>186</v>
       </c>
       <c r="K15" s="53" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>
@@ -4835,19 +4815,19 @@
         <v>44</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E16" s="22" t="s">
         <v>71</v>
       </c>
       <c r="F16" s="23">
-        <v>45106</v>
+        <v>45107</v>
       </c>
       <c r="G16" s="36" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H16" s="36" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I16" s="24" t="s">
         <v>188</v>
@@ -4863,13 +4843,13 @@
         <v>74</v>
       </c>
       <c r="N16" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O16" s="53" t="s">
         <v>74</v>
       </c>
       <c r="P16" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="26"/>
@@ -4878,7 +4858,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="105.75" hidden="1" thickBot="1">
+    <row r="17" spans="1:20" ht="105.75" thickBot="1">
       <c r="A17" s="20">
         <v>44</v>
       </c>
@@ -4909,7 +4889,7 @@
       <c r="N17" s="25"/>
       <c r="O17" s="25"/>
       <c r="P17" s="33" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="26"/>
@@ -4918,7 +4898,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="18" spans="1:20" ht="165.75" thickBot="1">
       <c r="A18" s="20">
         <v>52</v>
       </c>
@@ -4942,7 +4922,7 @@
         <v>186</v>
       </c>
       <c r="K18" s="33" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L18" s="34"/>
       <c r="M18" s="25"/>
@@ -4956,7 +4936,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="19" spans="1:20" ht="165.75" thickBot="1">
       <c r="A19" s="20">
         <v>53</v>
       </c>
@@ -4980,7 +4960,7 @@
         <v>186</v>
       </c>
       <c r="K19" s="33" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L19" s="34"/>
       <c r="M19" s="25"/>
@@ -4994,7 +4974,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="20" spans="1:20" ht="165.75" thickBot="1">
       <c r="A20" s="20">
         <v>54</v>
       </c>
@@ -5018,7 +4998,7 @@
         <v>186</v>
       </c>
       <c r="K20" s="33" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L20" s="34"/>
       <c r="M20" s="25"/>
@@ -5032,7 +5012,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="21" spans="1:20" ht="165.75" thickBot="1">
       <c r="A21" s="20">
         <v>55</v>
       </c>
@@ -5056,7 +5036,7 @@
         <v>186</v>
       </c>
       <c r="K21" s="33" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L21" s="34"/>
       <c r="M21" s="25"/>
@@ -5070,7 +5050,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="22" spans="1:20" ht="165.75" thickBot="1">
       <c r="A22" s="20">
         <v>56</v>
       </c>
@@ -5094,7 +5074,7 @@
         <v>186</v>
       </c>
       <c r="K22" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L22" s="34"/>
       <c r="M22" s="25"/>
@@ -5108,7 +5088,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="23" spans="1:20" ht="165.75" thickBot="1">
       <c r="A23" s="20">
         <v>57</v>
       </c>
@@ -5132,7 +5112,7 @@
         <v>186</v>
       </c>
       <c r="K23" s="33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L23" s="34"/>
       <c r="M23" s="25"/>
@@ -5146,7 +5126,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="24" spans="1:20" ht="165.75" thickBot="1">
       <c r="A24" s="20">
         <v>58</v>
       </c>
@@ -5170,7 +5150,7 @@
         <v>186</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L24" s="34"/>
       <c r="M24" s="25"/>
@@ -5184,7 +5164,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="25" spans="1:20" ht="165.75" thickBot="1">
       <c r="A25" s="20">
         <v>59</v>
       </c>
@@ -5208,7 +5188,7 @@
         <v>186</v>
       </c>
       <c r="K25" s="33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L25" s="34"/>
       <c r="M25" s="25"/>
@@ -5222,7 +5202,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="26" spans="1:20" ht="165.75" thickBot="1">
       <c r="A26" s="20">
         <v>60</v>
       </c>
@@ -5246,7 +5226,7 @@
         <v>186</v>
       </c>
       <c r="K26" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L26" s="34"/>
       <c r="M26" s="25"/>
@@ -5271,22 +5251,22 @@
         <v>44</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E27" s="22" t="s">
         <v>94</v>
       </c>
       <c r="F27" s="23">
-        <v>45106</v>
+        <v>45107</v>
       </c>
       <c r="G27" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="H27" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="I27" s="36" t="s">
         <v>249</v>
-      </c>
-      <c r="H27" s="36" t="s">
-        <v>250</v>
-      </c>
-      <c r="I27" s="36" t="s">
-        <v>251</v>
       </c>
       <c r="J27" s="33" t="s">
         <v>74</v>
@@ -5299,13 +5279,13 @@
         <v>74</v>
       </c>
       <c r="N27" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O27" s="33" t="s">
         <v>74</v>
       </c>
       <c r="P27" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="26"/>
@@ -5314,7 +5294,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="28" spans="1:20" ht="165.75" thickBot="1">
       <c r="A28" s="20">
         <v>62</v>
       </c>
@@ -5338,7 +5318,7 @@
         <v>186</v>
       </c>
       <c r="K28" s="33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L28" s="34"/>
       <c r="M28" s="25"/>
@@ -5369,7 +5349,7 @@
         <v>61</v>
       </c>
       <c r="F29" s="35">
-        <v>45106</v>
+        <v>45107</v>
       </c>
       <c r="G29" s="36" t="s">
         <v>252</v>
@@ -5396,7 +5376,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="195.75" hidden="1" thickBot="1">
+    <row r="30" spans="1:20" ht="195.75" thickBot="1">
       <c r="A30" s="40">
         <v>12</v>
       </c>
@@ -5420,7 +5400,7 @@
         <v>186</v>
       </c>
       <c r="K30" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L30" s="34"/>
       <c r="M30" s="33"/>
@@ -5434,7 +5414,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="195.75" hidden="1" thickBot="1">
+    <row r="31" spans="1:20" ht="195.75" thickBot="1">
       <c r="A31" s="40">
         <v>13</v>
       </c>
@@ -5458,7 +5438,7 @@
         <v>186</v>
       </c>
       <c r="K31" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L31" s="34"/>
       <c r="M31" s="33"/>
@@ -5472,7 +5452,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="195.75" hidden="1" thickBot="1">
+    <row r="32" spans="1:20" ht="195.75" thickBot="1">
       <c r="A32" s="40">
         <v>14</v>
       </c>
@@ -5496,7 +5476,7 @@
         <v>186</v>
       </c>
       <c r="K32" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L32" s="34"/>
       <c r="M32" s="33"/>
@@ -5510,7 +5490,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="210.75" hidden="1" thickBot="1">
+    <row r="33" spans="1:20" ht="210.75" thickBot="1">
       <c r="A33" s="40">
         <v>31</v>
       </c>
@@ -5534,7 +5514,7 @@
         <v>186</v>
       </c>
       <c r="K33" s="53" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L33" s="34"/>
       <c r="M33" s="34"/>
@@ -5559,19 +5539,19 @@
         <v>48</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E34" s="39" t="s">
         <v>193</v>
       </c>
       <c r="F34" s="23">
-        <v>45106</v>
+        <v>45107</v>
       </c>
       <c r="G34" s="36" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="H34" s="36" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="I34" s="24" t="s">
         <v>188</v>
@@ -5587,13 +5567,13 @@
         <v>74</v>
       </c>
       <c r="N34" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O34" s="53" t="s">
         <v>74</v>
       </c>
       <c r="P34" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="26"/>
@@ -5602,7 +5582,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="105.75" hidden="1" thickBot="1">
+    <row r="35" spans="1:20" ht="105.75" thickBot="1">
       <c r="A35" s="40">
         <v>47</v>
       </c>
@@ -5633,7 +5613,7 @@
       <c r="N35" s="25"/>
       <c r="O35" s="25"/>
       <c r="P35" s="33" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q35" s="25"/>
       <c r="R35" s="26"/>
@@ -5642,7 +5622,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="180.75" hidden="1" thickBot="1">
+    <row r="36" spans="1:20" ht="180.75" thickBot="1">
       <c r="A36" s="40">
         <v>75</v>
       </c>
@@ -5666,7 +5646,7 @@
         <v>186</v>
       </c>
       <c r="K36" s="33" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L36" s="33"/>
       <c r="M36" s="33"/>
@@ -5680,7 +5660,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="37" spans="1:20" ht="165.75" thickBot="1">
       <c r="A37" s="40">
         <v>76</v>
       </c>
@@ -5704,7 +5684,7 @@
         <v>186</v>
       </c>
       <c r="K37" s="33" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L37" s="33"/>
       <c r="M37" s="33"/>
@@ -5718,7 +5698,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="38" spans="1:20" ht="150.75" thickBot="1">
       <c r="A38" s="40">
         <v>77</v>
       </c>
@@ -5742,7 +5722,7 @@
         <v>186</v>
       </c>
       <c r="K38" s="33" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L38" s="33"/>
       <c r="M38" s="33"/>
@@ -5756,7 +5736,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="39" spans="1:20" ht="150.75" thickBot="1">
       <c r="A39" s="40">
         <v>78</v>
       </c>
@@ -5780,7 +5760,7 @@
         <v>186</v>
       </c>
       <c r="K39" s="33" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L39" s="33"/>
       <c r="M39" s="33"/>
@@ -5794,7 +5774,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="40" spans="1:20" ht="165.75" thickBot="1">
       <c r="A40" s="40">
         <v>79</v>
       </c>
@@ -5818,7 +5798,7 @@
         <v>186</v>
       </c>
       <c r="K40" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L40" s="33"/>
       <c r="M40" s="33"/>
@@ -5832,7 +5812,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="41" spans="1:20" ht="165.75" thickBot="1">
       <c r="A41" s="40">
         <v>80</v>
       </c>
@@ -5856,7 +5836,7 @@
         <v>186</v>
       </c>
       <c r="K41" s="33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L41" s="33"/>
       <c r="M41" s="33"/>
@@ -5870,7 +5850,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="42" spans="1:20" ht="165.75" thickBot="1">
       <c r="A42" s="40">
         <v>81</v>
       </c>
@@ -5894,7 +5874,7 @@
         <v>186</v>
       </c>
       <c r="K42" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L42" s="25"/>
       <c r="M42" s="25"/>
@@ -5908,7 +5888,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="43" spans="1:20" ht="165.75" thickBot="1">
       <c r="A43" s="40">
         <v>82</v>
       </c>
@@ -5932,7 +5912,7 @@
         <v>186</v>
       </c>
       <c r="K43" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L43" s="33"/>
       <c r="M43" s="33"/>
@@ -5946,7 +5926,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="44" spans="1:20" ht="150.75" thickBot="1">
       <c r="A44" s="40">
         <v>83</v>
       </c>
@@ -5970,7 +5950,7 @@
         <v>186</v>
       </c>
       <c r="K44" s="33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L44" s="33"/>
       <c r="M44" s="33"/>
@@ -5995,22 +5975,22 @@
         <v>48</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E45" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F45" s="46">
-        <v>45106</v>
+        <v>45107</v>
       </c>
       <c r="G45" s="46" t="s">
+        <v>255</v>
+      </c>
+      <c r="H45" s="71" t="s">
+        <v>256</v>
+      </c>
+      <c r="I45" s="39" t="s">
         <v>257</v>
-      </c>
-      <c r="H45" s="72" t="s">
-        <v>255</v>
-      </c>
-      <c r="I45" s="73" t="s">
-        <v>256</v>
       </c>
       <c r="J45" s="47" t="s">
         <v>74</v>
@@ -6040,7 +6020,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="165" hidden="1">
+    <row r="46" spans="1:20" ht="165.75" thickBot="1">
       <c r="A46" s="40">
         <v>85</v>
       </c>
@@ -6064,7 +6044,7 @@
         <v>186</v>
       </c>
       <c r="K46" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L46" s="33"/>
       <c r="M46" s="33"/>
@@ -6078,7 +6058,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="165" hidden="1">
+    <row r="47" spans="1:20" ht="165.75" thickBot="1">
       <c r="A47" s="40">
         <v>86</v>
       </c>
@@ -6102,7 +6082,7 @@
         <v>186</v>
       </c>
       <c r="K47" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L47" s="33"/>
       <c r="M47" s="33"/>
@@ -6116,7 +6096,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="180" hidden="1">
+    <row r="48" spans="1:20" ht="180.75" thickBot="1">
       <c r="A48" s="40">
         <v>87</v>
       </c>
@@ -6140,7 +6120,7 @@
         <v>186</v>
       </c>
       <c r="K48" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L48" s="33"/>
       <c r="M48" s="33"/>
@@ -6154,7 +6134,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="165" hidden="1">
+    <row r="49" spans="1:20" ht="165.75" thickBot="1">
       <c r="A49" s="40">
         <v>88</v>
       </c>
@@ -6178,7 +6158,7 @@
         <v>186</v>
       </c>
       <c r="K49" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L49" s="33"/>
       <c r="M49" s="33"/>
@@ -6192,7 +6172,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="150" hidden="1">
+    <row r="50" spans="1:20" ht="150.75" thickBot="1">
       <c r="A50" s="40">
         <v>89</v>
       </c>
@@ -6216,7 +6196,7 @@
         <v>186</v>
       </c>
       <c r="K50" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L50" s="33"/>
       <c r="M50" s="33"/>
@@ -6230,7 +6210,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="150" hidden="1">
+    <row r="51" spans="1:20" ht="150.75" thickBot="1">
       <c r="A51" s="40">
         <v>90</v>
       </c>
@@ -6254,7 +6234,7 @@
         <v>186</v>
       </c>
       <c r="K51" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L51" s="33"/>
       <c r="M51" s="33"/>
@@ -6268,7 +6248,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="165" hidden="1">
+    <row r="52" spans="1:20" ht="165.75" thickBot="1">
       <c r="A52" s="40">
         <v>91</v>
       </c>
@@ -6292,7 +6272,7 @@
         <v>186</v>
       </c>
       <c r="K52" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L52" s="33"/>
       <c r="M52" s="33"/>
@@ -6306,7 +6286,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="165" hidden="1">
+    <row r="53" spans="1:20" ht="165.75" thickBot="1">
       <c r="A53" s="40">
         <v>92</v>
       </c>
@@ -6330,7 +6310,7 @@
         <v>186</v>
       </c>
       <c r="K53" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L53" s="33"/>
       <c r="M53" s="33"/>
@@ -6344,7 +6324,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="165" hidden="1">
+    <row r="54" spans="1:20" ht="165.75" thickBot="1">
       <c r="A54" s="40">
         <v>93</v>
       </c>
@@ -6368,7 +6348,7 @@
         <v>186</v>
       </c>
       <c r="K54" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L54" s="33"/>
       <c r="M54" s="33"/>
@@ -6382,7 +6362,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="210" hidden="1">
+    <row r="55" spans="1:20" ht="210">
       <c r="A55" s="20">
         <v>191</v>
       </c>
@@ -6406,7 +6386,7 @@
         <v>186</v>
       </c>
       <c r="K55" s="33" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L55" s="25"/>
       <c r="M55" s="25"/>
@@ -6421,10 +6401,10 @@
       </c>
     </row>
     <row r="56" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F56" s="69"/>
+      <c r="F56" s="55"/>
       <c r="G56" s="12"/>
-      <c r="H56" s="71"/>
-      <c r="I56" s="69"/>
+      <c r="H56" s="55"/>
+      <c r="I56" s="55"/>
       <c r="J56" s="13"/>
       <c r="K56" s="13"/>
       <c r="L56" s="13"/>
@@ -14878,13 +14858,7 @@
       <c r="T606" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T55" xr:uid="{00000000-0009-0000-0000-000002000000}">
-    <filterColumn colId="5">
-      <filters>
-        <dateGroupItem year="2023" month="6" day="29" dateTimeGrouping="day"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A9:T55" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>

</xml_diff>